<commit_message>
UnoApiXmlTest: merge parseExport from ChartTest
Reuse existing mechanism to handle chart file names in tests.
See https://lists.freedesktop.org/archives/libreoffice/2023-February/089995.html
and 0236a09d73b49ee689e42814bd4c2a8da4d570ae
"fix chart export tests correctly
we have a static counter that increments chart export file names. So
only the first exported file gets the file name chart1.xml and all the
following charts are incremented by one even if they are in a different
file."

Also add an assert to warn developers only 1 chart is allow per sample
document when parsing them.
Adapt a few tests to follow this rule and change file document
from testMultipleChart.docx to testExternalData.docx because
the name was misleading

Change-Id: Id7282049796f2b05492ab70b50c80065a99439be
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/148065
Tested-by: Jenkins
Reviewed-by: Xisco Fauli <xiscofauli@libreoffice.org>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/chart_pie2007.xlsx
+++ b/chart2/qa/extras/data/xlsx/chart_pie2007.xlsx
@@ -180,218 +180,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Pie Chart with user defined colors</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Pie sales data</c:v>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="5ABA10"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FE110E"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="CA5C05"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Apple</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cherry</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Pecan</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Pie Chart with segment rotation</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Pie sales data</c:v>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Apple</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Cherry</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Pecan</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="90"/>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -419,66 +207,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>

</xml_diff>